<commit_message>
Updated EP_GeneList.xlsx changed MHS VCEP name "ClinGen Malignant Hyperthermia Susceptibility Variant Curation Expert Panel,ClinGen" changed Rett ANgelman to "ClinGen Rett and Angelman-like Disorders Variant Curation Expert Panel, ClinGen"
</commit_message>
<xml_diff>
--- a/EP_GeneList.xlsx
+++ b/EP_GeneList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toneill/dev/git/clinvar-ep-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9EB4F5-5E33-B84B-A15C-E8298B19A4A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BFB8ED-5D20-FB4B-B6AB-E5DCCB00DB3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t>MECP2</t>
   </si>
   <si>
-    <t>Rett_Angelman-like Disorders</t>
-  </si>
-  <si>
     <t>CDKL5</t>
   </si>
   <si>
@@ -523,9 +520,6 @@
   </si>
   <si>
     <t>RYR1</t>
-  </si>
-  <si>
-    <t>MHS</t>
   </si>
   <si>
     <t>CACNA1S</t>
@@ -805,6 +799,12 @@
   </si>
   <si>
     <t>CACNA1F</t>
+  </si>
+  <si>
+    <t>ClinGen Rett and Angelman-like Disorders Variant Curation Expert Panel, ClinGen</t>
+  </si>
+  <si>
+    <t>ClinGen Malignant Hyperthermia Susceptibility Variant Curation Expert Panel,ClinGen</t>
   </si>
 </sst>
 </file>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="A178" sqref="A1:Z221"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1253,10 +1253,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1785,10 +1785,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1817,10 +1817,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1849,10 +1849,10 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1915,10 +1915,10 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1947,10 +1947,10 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1979,10 +1979,10 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2011,10 +2011,10 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2075,10 +2075,10 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2107,10 +2107,10 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2139,10 +2139,10 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -2267,10 +2267,10 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -2299,10 +2299,10 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -2331,10 +2331,10 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -2363,10 +2363,10 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -2395,10 +2395,10 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -2427,10 +2427,10 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2491,10 +2491,10 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2523,10 +2523,10 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2555,10 +2555,10 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -2587,10 +2587,10 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2619,10 +2619,10 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -2651,10 +2651,10 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -2683,10 +2683,10 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -2715,10 +2715,10 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -2747,10 +2747,10 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -2779,10 +2779,10 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -2811,10 +2811,10 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -2843,10 +2843,10 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2875,10 +2875,10 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2978,7 +2978,7 @@
         <v>65</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -3010,7 +3010,7 @@
         <v>66</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -3042,7 +3042,7 @@
         <v>67</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -3103,10 +3103,10 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -3135,10 +3135,10 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -3199,10 +3199,10 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -3231,10 +3231,10 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -3569,10 +3569,10 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1">
       <c r="A76" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -3601,10 +3601,10 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -3633,10 +3633,10 @@
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
@@ -3665,10 +3665,10 @@
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -3697,10 +3697,10 @@
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3729,10 +3729,10 @@
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -3761,10 +3761,10 @@
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
@@ -3793,10 +3793,10 @@
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3828,7 +3828,7 @@
         <v>77</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -3860,7 +3860,7 @@
         <v>78</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -3892,7 +3892,7 @@
         <v>79</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -3924,7 +3924,7 @@
         <v>80</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
@@ -3956,7 +3956,7 @@
         <v>81</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
@@ -3988,7 +3988,7 @@
         <v>82</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -4020,7 +4020,7 @@
         <v>83</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
@@ -4049,10 +4049,10 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
@@ -4081,10 +4081,10 @@
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -4113,10 +4113,10 @@
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -4213,7 +4213,7 @@
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>14</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="98" spans="1:26" ht="15.75" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>14</v>
@@ -4313,7 +4313,7 @@
     </row>
     <row r="99" spans="1:26" ht="15.75" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>14</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="100" spans="1:26" ht="15.75" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>14</v>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="101" spans="1:26" ht="15.75" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>14</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="102" spans="1:26" ht="15.75" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>14</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="103" spans="1:26" ht="15.75" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>14</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="104" spans="1:26" ht="15.75" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>14</v>
@@ -4537,10 +4537,10 @@
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1">
       <c r="A106" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -4569,10 +4569,10 @@
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -4601,10 +4601,10 @@
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -4633,10 +4633,10 @@
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -4665,10 +4665,10 @@
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
@@ -4697,10 +4697,10 @@
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
@@ -4729,10 +4729,10 @@
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1">
       <c r="A112" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
@@ -4761,10 +4761,10 @@
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
@@ -4793,10 +4793,10 @@
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
@@ -4825,10 +4825,10 @@
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
@@ -4857,10 +4857,10 @@
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1">
       <c r="A116" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -4889,10 +4889,10 @@
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
@@ -4921,10 +4921,10 @@
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
@@ -4953,10 +4953,10 @@
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
@@ -4985,10 +4985,10 @@
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
@@ -5017,10 +5017,10 @@
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
@@ -5049,10 +5049,10 @@
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
@@ -5081,10 +5081,10 @@
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
@@ -5215,10 +5215,10 @@
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>166</v>
+        <v>259</v>
       </c>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -5247,10 +5247,10 @@
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>166</v>
+        <v>259</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -5279,10 +5279,10 @@
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
@@ -5311,10 +5311,10 @@
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
@@ -5343,10 +5343,10 @@
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -5375,10 +5375,10 @@
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
@@ -5897,7 +5897,7 @@
     </row>
     <row r="148" spans="1:26" ht="15.75" customHeight="1">
       <c r="A148" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>72</v>
@@ -5931,10 +5931,10 @@
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1">
       <c r="A149" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
@@ -5963,10 +5963,10 @@
     </row>
     <row r="150" spans="1:26" ht="15.75" customHeight="1">
       <c r="A150" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
@@ -5995,10 +5995,10 @@
     </row>
     <row r="151" spans="1:26" ht="15.75" customHeight="1">
       <c r="A151" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
@@ -6027,10 +6027,10 @@
     </row>
     <row r="152" spans="1:26" ht="15.75" customHeight="1">
       <c r="A152" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
@@ -6059,10 +6059,10 @@
     </row>
     <row r="153" spans="1:26" ht="15.75" customHeight="1">
       <c r="A153" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
@@ -6091,10 +6091,10 @@
     </row>
     <row r="154" spans="1:26" ht="15.75" customHeight="1">
       <c r="A154" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
@@ -6123,10 +6123,10 @@
     </row>
     <row r="155" spans="1:26" ht="15.75" customHeight="1">
       <c r="A155" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
@@ -6189,10 +6189,10 @@
     </row>
     <row r="157" spans="1:26" ht="15.75" customHeight="1">
       <c r="A157" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
@@ -6221,10 +6221,10 @@
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1">
       <c r="A158" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
@@ -6253,10 +6253,10 @@
     </row>
     <row r="159" spans="1:26" ht="15.75" customHeight="1">
       <c r="A159" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
@@ -6285,10 +6285,10 @@
     </row>
     <row r="160" spans="1:26" ht="15.75" customHeight="1">
       <c r="A160" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
@@ -6317,10 +6317,10 @@
     </row>
     <row r="161" spans="1:26" ht="15.75" customHeight="1">
       <c r="A161" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
@@ -6349,10 +6349,10 @@
     </row>
     <row r="162" spans="1:26" ht="15.75" customHeight="1">
       <c r="A162" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
@@ -6381,10 +6381,10 @@
     </row>
     <row r="163" spans="1:26" ht="15.75" customHeight="1">
       <c r="A163" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
@@ -6413,10 +6413,10 @@
     </row>
     <row r="164" spans="1:26" ht="15.75" customHeight="1">
       <c r="A164" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
@@ -6445,10 +6445,10 @@
     </row>
     <row r="165" spans="1:26" ht="15.75" customHeight="1">
       <c r="A165" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
@@ -6477,10 +6477,10 @@
     </row>
     <row r="166" spans="1:26" ht="15.75" customHeight="1">
       <c r="A166" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -6509,10 +6509,10 @@
     </row>
     <row r="167" spans="1:26" ht="15.75" customHeight="1">
       <c r="A167" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
@@ -6541,10 +6541,10 @@
     </row>
     <row r="168" spans="1:26" ht="15.75" customHeight="1">
       <c r="A168" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
@@ -6573,10 +6573,10 @@
     </row>
     <row r="169" spans="1:26" ht="15.75" customHeight="1">
       <c r="A169" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
@@ -6605,10 +6605,10 @@
     </row>
     <row r="170" spans="1:26" ht="15.75" customHeight="1">
       <c r="A170" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
@@ -6637,10 +6637,10 @@
     </row>
     <row r="171" spans="1:26" ht="15.75" customHeight="1">
       <c r="A171" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
@@ -6669,10 +6669,10 @@
     </row>
     <row r="172" spans="1:26" ht="15.75" customHeight="1">
       <c r="A172" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
@@ -6701,10 +6701,10 @@
     </row>
     <row r="173" spans="1:26" ht="15.75" customHeight="1">
       <c r="A173" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
@@ -6733,10 +6733,10 @@
     </row>
     <row r="174" spans="1:26" ht="15.75" customHeight="1">
       <c r="A174" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
@@ -6765,10 +6765,10 @@
     </row>
     <row r="175" spans="1:26" ht="15.75" customHeight="1">
       <c r="A175" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
@@ -6797,10 +6797,10 @@
     </row>
     <row r="176" spans="1:26" ht="15.75" customHeight="1">
       <c r="A176" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
@@ -6829,10 +6829,10 @@
     </row>
     <row r="177" spans="1:26" ht="15.75" customHeight="1">
       <c r="A177" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B177" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B177" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C177" s="5">
         <v>507662</v>
@@ -6863,10 +6863,10 @@
     </row>
     <row r="178" spans="1:26" ht="15.75" customHeight="1">
       <c r="A178" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C178" s="5">
         <v>507662</v>
@@ -6897,10 +6897,10 @@
     </row>
     <row r="179" spans="1:26" ht="15.75" customHeight="1">
       <c r="A179" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C179" s="5">
         <v>507662</v>
@@ -6931,10 +6931,10 @@
     </row>
     <row r="180" spans="1:26" ht="15.75" customHeight="1">
       <c r="A180" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C180" s="5">
         <v>507662</v>
@@ -6965,10 +6965,10 @@
     </row>
     <row r="181" spans="1:26" ht="15.75" customHeight="1">
       <c r="A181" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C181" s="5">
         <v>507662</v>
@@ -7339,7 +7339,7 @@
     </row>
     <row r="192" spans="1:26" ht="15.75" customHeight="1">
       <c r="A192" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B192" s="4" t="s">
         <v>4</v>
@@ -7373,7 +7373,7 @@
     </row>
     <row r="193" spans="1:26" ht="15.75" customHeight="1">
       <c r="A193" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B193" s="4" t="s">
         <v>4</v>
@@ -7407,7 +7407,7 @@
     </row>
     <row r="194" spans="1:26" ht="15.75" customHeight="1">
       <c r="A194" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B194" s="4" t="s">
         <v>4</v>
@@ -7444,7 +7444,7 @@
         <v>89</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
@@ -7473,10 +7473,10 @@
     </row>
     <row r="196" spans="1:26" ht="15.75" customHeight="1">
       <c r="A196" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
@@ -7505,10 +7505,10 @@
     </row>
     <row r="197" spans="1:26" ht="15.75" customHeight="1">
       <c r="A197" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
@@ -7537,10 +7537,10 @@
     </row>
     <row r="198" spans="1:26" ht="15.75" customHeight="1">
       <c r="A198" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C198" s="4"/>
       <c r="D198" s="4"/>
@@ -7569,10 +7569,10 @@
     </row>
     <row r="199" spans="1:26" ht="15.75" customHeight="1">
       <c r="A199" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
@@ -7601,10 +7601,10 @@
     </row>
     <row r="200" spans="1:26" ht="15.75" customHeight="1">
       <c r="A200" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C200" s="4"/>
       <c r="D200" s="4"/>
@@ -7633,10 +7633,10 @@
     </row>
     <row r="201" spans="1:26" ht="15.75" customHeight="1">
       <c r="A201" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C201" s="4"/>
       <c r="D201" s="4"/>
@@ -7665,10 +7665,10 @@
     </row>
     <row r="202" spans="1:26" ht="15.75" customHeight="1">
       <c r="A202" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
@@ -7697,10 +7697,10 @@
     </row>
     <row r="203" spans="1:26" ht="15.75" customHeight="1">
       <c r="A203" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
@@ -7729,10 +7729,10 @@
     </row>
     <row r="204" spans="1:26" ht="15.75" customHeight="1">
       <c r="A204" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
@@ -7761,10 +7761,10 @@
     </row>
     <row r="205" spans="1:26" ht="15.75" customHeight="1">
       <c r="A205" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
@@ -7793,10 +7793,10 @@
     </row>
     <row r="206" spans="1:26" ht="15.75" customHeight="1">
       <c r="A206" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C206" s="4"/>
       <c r="D206" s="4"/>
@@ -7825,10 +7825,10 @@
     </row>
     <row r="207" spans="1:26" ht="15.75" customHeight="1">
       <c r="A207" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
@@ -7857,10 +7857,10 @@
     </row>
     <row r="208" spans="1:26" ht="15.75" customHeight="1">
       <c r="A208" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C208" s="4"/>
       <c r="D208" s="4"/>
@@ -7889,10 +7889,10 @@
     </row>
     <row r="209" spans="1:26" ht="15.75" customHeight="1">
       <c r="A209" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C209" s="4"/>
       <c r="D209" s="4"/>
@@ -7921,10 +7921,10 @@
     </row>
     <row r="210" spans="1:26" ht="15.75" customHeight="1">
       <c r="A210" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C210" s="4"/>
       <c r="D210" s="4"/>
@@ -7953,10 +7953,10 @@
     </row>
     <row r="211" spans="1:26" ht="15.75" customHeight="1">
       <c r="A211" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C211" s="4"/>
       <c r="D211" s="4"/>
@@ -8051,10 +8051,10 @@
     </row>
     <row r="214" spans="1:26" ht="15.75" customHeight="1">
       <c r="A214" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
@@ -8083,10 +8083,10 @@
     </row>
     <row r="215" spans="1:26" ht="15.75" customHeight="1">
       <c r="A215" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
@@ -8115,10 +8115,10 @@
     </row>
     <row r="216" spans="1:26" ht="15.75" customHeight="1">
       <c r="A216" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C216" s="4"/>
       <c r="D216" s="4"/>
@@ -8147,10 +8147,10 @@
     </row>
     <row r="217" spans="1:26" ht="15.75" customHeight="1">
       <c r="A217" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C217" s="4"/>
       <c r="D217" s="4"/>
@@ -8179,10 +8179,10 @@
     </row>
     <row r="218" spans="1:26" ht="15.75" customHeight="1">
       <c r="A218" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C218" s="4"/>
       <c r="D218" s="4"/>
@@ -8211,10 +8211,10 @@
     </row>
     <row r="219" spans="1:26" ht="15.75" customHeight="1">
       <c r="A219" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C219" s="4"/>
       <c r="D219" s="4"/>
@@ -8243,10 +8243,10 @@
     </row>
     <row r="220" spans="1:26" ht="15.75" customHeight="1">
       <c r="A220" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C220" s="4"/>
       <c r="D220" s="4"/>
@@ -8275,10 +8275,10 @@
     </row>
     <row r="221" spans="1:26" ht="15.75" customHeight="1">
       <c r="A221" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C221" s="4"/>
       <c r="D221" s="4"/>

</xml_diff>